<commit_message>
Published state of ETDataset on 26th of March 2019
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/industry/industry_chp_combined_cycle_gas_power_fuelmix.central_producer.xlsx
+++ b/nodes_source_analyses/industry/industry_chp_combined_cycle_gas_power_fuelmix.central_producer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marliekeverweij/Projects/etdataset/nodes_source_analyses/industry/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexander/Git/etdataset/nodes_source_analyses/industry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AE7BD2-2B0E-C746-815A-9F1BAB1923BA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA0A514-9473-1F4A-B91E-0F36B8EFCE64}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="762" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -37,10 +37,16 @@
     <definedName name="Wp_to_kWp">#REF!</definedName>
     <definedName name="WP_to_MWp">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -50,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="187">
   <si>
     <t>Source</t>
   </si>
@@ -577,9 +583,6 @@
   </si>
   <si>
     <t>yr</t>
-  </si>
-  <si>
-    <t>Ennergymatters</t>
   </si>
   <si>
     <t>p.1</t>
@@ -1634,7 +1637,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="34" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="200">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1984,6 +1987,7 @@
     <xf numFmtId="0" fontId="32" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="254">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2875,12 +2879,12 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.5" style="26" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="44.1640625" style="18" customWidth="1"/>
-    <col min="4" max="16384" width="10.6640625" style="18"/>
+    <col min="1" max="1" width="3.42578125" style="26" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" style="18" customWidth="1"/>
+    <col min="4" max="16384" width="10.7109375" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="24" customFormat="1">
@@ -2906,7 +2910,7 @@
         <v>18</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3054,23 +3058,23 @@
   </sheetPr>
   <dimension ref="B1:K40"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="34" customWidth="1"/>
-    <col min="2" max="2" width="3.6640625" style="34" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="34" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" style="34" customWidth="1"/>
     <col min="3" max="3" width="46" style="34" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="34" customWidth="1"/>
-    <col min="5" max="5" width="17.5" style="34" customWidth="1"/>
-    <col min="6" max="6" width="4.5" style="34" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="34" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="34" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" style="34" customWidth="1"/>
     <col min="7" max="7" width="45" style="34" customWidth="1"/>
-    <col min="8" max="8" width="5.1640625" style="34" customWidth="1"/>
-    <col min="9" max="9" width="51.5" style="34" customWidth="1"/>
-    <col min="10" max="10" width="5.5" style="34" customWidth="1"/>
-    <col min="11" max="16384" width="10.6640625" style="34"/>
+    <col min="8" max="8" width="5.140625" style="34" customWidth="1"/>
+    <col min="9" max="9" width="51.42578125" style="34" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" style="34" customWidth="1"/>
+    <col min="11" max="16384" width="10.7109375" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11">
@@ -3081,7 +3085,7 @@
     </row>
     <row r="2" spans="2:11">
       <c r="B2" s="190" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C2" s="191"/>
       <c r="D2" s="191"/>
@@ -3180,7 +3184,7 @@
       <c r="G10" s="33"/>
       <c r="H10" s="27"/>
       <c r="I10" s="188" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J10" s="42"/>
     </row>
@@ -3200,7 +3204,7 @@
       <c r="G11" s="33"/>
       <c r="H11" s="27"/>
       <c r="I11" s="188" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J11" s="42"/>
     </row>
@@ -3302,7 +3306,7 @@
       </c>
       <c r="H16" s="33"/>
       <c r="I16" s="188" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J16" s="129"/>
     </row>
@@ -3324,7 +3328,7 @@
       </c>
       <c r="H17" s="33"/>
       <c r="I17" s="188" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J17" s="129"/>
     </row>
@@ -3455,7 +3459,7 @@
       </c>
       <c r="H24" s="33"/>
       <c r="I24" s="188" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J24" s="129"/>
     </row>
@@ -3477,7 +3481,7 @@
       </c>
       <c r="H25" s="33"/>
       <c r="I25" s="188" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J25" s="129"/>
     </row>
@@ -3576,7 +3580,7 @@
       </c>
       <c r="E31" s="44">
         <f>'Research data'!G11</f>
-        <v>0.1</v>
+        <v>0.12968399999999999</v>
       </c>
       <c r="F31" s="33"/>
       <c r="G31" s="33" t="s">
@@ -3628,7 +3632,7 @@
       </c>
       <c r="H33" s="33"/>
       <c r="I33" s="150" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J33" s="129"/>
     </row>
@@ -3763,29 +3767,29 @@
   </sheetPr>
   <dimension ref="B1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="3.5" style="73" customWidth="1"/>
-    <col min="3" max="3" width="35.83203125" style="73" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="73" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" style="73" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="73" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="73" customWidth="1"/>
-    <col min="8" max="8" width="2.6640625" style="74" customWidth="1"/>
-    <col min="9" max="9" width="9.83203125" style="74" customWidth="1"/>
+    <col min="1" max="2" width="3.42578125" style="73" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="73" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="73" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="73" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="73" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="73" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" style="74" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" style="74" customWidth="1"/>
     <col min="10" max="10" width="3" style="74" customWidth="1"/>
-    <col min="11" max="11" width="10.5" style="74" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" style="74" customWidth="1"/>
     <col min="12" max="12" width="3" style="74" customWidth="1"/>
-    <col min="13" max="13" width="8.6640625" style="74" customWidth="1"/>
-    <col min="14" max="14" width="3.33203125" style="74" customWidth="1"/>
-    <col min="15" max="15" width="8.5" style="74" customWidth="1"/>
-    <col min="16" max="16" width="2.6640625" style="74" customWidth="1"/>
-    <col min="17" max="17" width="110.5" style="73" customWidth="1"/>
-    <col min="18" max="16384" width="10.6640625" style="73"/>
+    <col min="13" max="13" width="8.7109375" style="74" customWidth="1"/>
+    <col min="14" max="14" width="3.28515625" style="74" customWidth="1"/>
+    <col min="15" max="15" width="8.42578125" style="74" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" style="74" customWidth="1"/>
+    <col min="17" max="17" width="110.42578125" style="73" customWidth="1"/>
+    <col min="18" max="16384" width="10.7109375" style="73"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="17" thickBot="1"/>
@@ -3826,7 +3830,7 @@
       </c>
       <c r="J3" s="67"/>
       <c r="K3" s="67" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L3" s="67"/>
       <c r="M3" s="67" t="s">
@@ -3890,7 +3894,7 @@
         <v>69</v>
       </c>
       <c r="G6" s="84">
-        <f>ROUND(100,0)</f>
+        <f>I6</f>
         <v>100</v>
       </c>
       <c r="H6" s="80"/>
@@ -3908,7 +3912,7 @@
     <row r="7" spans="2:17" s="164" customFormat="1" ht="17" thickBot="1">
       <c r="B7" s="168"/>
       <c r="C7" s="172" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D7" s="173" t="s">
         <v>3</v>
@@ -3934,13 +3938,13 @@
       <c r="O7" s="178"/>
       <c r="P7" s="178"/>
       <c r="Q7" s="179" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="2:17" s="164" customFormat="1" ht="17" thickBot="1">
       <c r="B8" s="168"/>
       <c r="C8" s="172" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D8" s="173" t="s">
         <v>3</v>
@@ -3966,7 +3970,7 @@
       <c r="O8" s="178"/>
       <c r="P8" s="178"/>
       <c r="Q8" s="179" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="2:17">
@@ -4017,7 +4021,8 @@
         <v>4</v>
       </c>
       <c r="G11" s="93">
-        <v>0.1</v>
+        <f>O11</f>
+        <v>0.12968399999999999</v>
       </c>
       <c r="H11" s="87"/>
       <c r="I11" s="87"/>
@@ -4045,7 +4050,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="93">
-        <f>ROUND(2,0)</f>
+        <f>ROUND(M12,0)</f>
         <v>2</v>
       </c>
       <c r="H12" s="88"/>
@@ -4075,7 +4080,7 @@
         <v>2</v>
       </c>
       <c r="G13" s="96">
-        <f>ROUND(25,0)</f>
+        <f>M13</f>
         <v>25</v>
       </c>
       <c r="H13" s="88"/>
@@ -4191,7 +4196,7 @@
     <row r="18" spans="2:17" ht="17" thickBot="1">
       <c r="B18" s="78"/>
       <c r="C18" s="165" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D18" s="29"/>
       <c r="E18" s="29"/>
@@ -4245,7 +4250,7 @@
       <c r="O19" s="94"/>
       <c r="P19" s="87"/>
       <c r="Q19" s="166" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="2:17" ht="17" thickBot="1">
@@ -4269,7 +4274,7 @@
       <c r="O20" s="94"/>
       <c r="P20" s="87"/>
       <c r="Q20" s="167" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="2:17" ht="17" thickBot="1">
@@ -4299,7 +4304,7 @@
       <c r="O21" s="94"/>
       <c r="P21" s="87"/>
       <c r="Q21" s="167" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="2:17" ht="17" thickBot="1">
@@ -4326,7 +4331,7 @@
       <c r="O22" s="94"/>
       <c r="P22" s="87"/>
       <c r="Q22" s="167" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="2:17" ht="17" thickBot="1">
@@ -4384,7 +4389,7 @@
       <c r="O24" s="85"/>
       <c r="P24" s="85"/>
       <c r="Q24" s="167" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="2:17" ht="17" thickBot="1">
@@ -4432,18 +4437,18 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="33.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="33.140625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="46" customWidth="1"/>
-    <col min="2" max="2" width="3.5" style="46" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" style="46" customWidth="1"/>
-    <col min="4" max="4" width="3.1640625" style="46" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" style="46" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="46" customWidth="1"/>
-    <col min="7" max="9" width="12.1640625" style="46" customWidth="1"/>
-    <col min="10" max="10" width="35.1640625" style="47" customWidth="1"/>
-    <col min="11" max="11" width="130.33203125" style="46" customWidth="1"/>
-    <col min="12" max="16384" width="33.1640625" style="46"/>
+    <col min="1" max="1" width="3.28515625" style="46" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" style="46" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" style="46" customWidth="1"/>
+    <col min="4" max="4" width="3.140625" style="46" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" style="46" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="46" customWidth="1"/>
+    <col min="7" max="9" width="12.140625" style="46" customWidth="1"/>
+    <col min="10" max="10" width="35.140625" style="47" customWidth="1"/>
+    <col min="11" max="11" width="130.28515625" style="46" customWidth="1"/>
+    <col min="12" max="16384" width="33.140625" style="46"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="17" thickBot="1"/>
@@ -4507,7 +4512,7 @@
         <v>62</v>
       </c>
       <c r="J5" s="58" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K5" s="57" t="s">
         <v>16</v>
@@ -4543,10 +4548,10 @@
       </c>
       <c r="I7" s="55"/>
       <c r="J7" s="55" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K7" s="70" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="2:11">
@@ -4589,7 +4594,7 @@
       <c r="J10" s="55"/>
       <c r="K10" s="71"/>
     </row>
-    <row r="11" spans="2:11" ht="32">
+    <row r="11" spans="2:11" ht="17">
       <c r="B11" s="51"/>
       <c r="C11" s="59"/>
       <c r="D11" s="64"/>
@@ -4607,7 +4612,7 @@
       </c>
       <c r="I11" s="62"/>
       <c r="J11" s="62" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K11" s="59"/>
     </row>
@@ -4656,7 +4661,7 @@
       <c r="C15" s="59"/>
       <c r="D15" s="59"/>
       <c r="E15" s="59" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F15" s="54" t="s">
         <v>70</v>
@@ -4669,10 +4674,10 @@
       </c>
       <c r="I15" s="54"/>
       <c r="J15" s="55" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K15" s="63" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="2:11">
@@ -4821,17 +4826,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:Q117"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" style="148" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" style="148" customWidth="1"/>
     <col min="2" max="2" width="4" style="148" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="148" customWidth="1"/>
-    <col min="4" max="5" width="13.83203125" style="148" customWidth="1"/>
-    <col min="6" max="16384" width="10.6640625" style="148"/>
+    <col min="3" max="3" width="13.42578125" style="148" customWidth="1"/>
+    <col min="4" max="5" width="13.85546875" style="148" customWidth="1"/>
+    <col min="6" max="16384" width="10.7109375" style="148"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="17" thickBot="1"/>
@@ -4909,8 +4914,8 @@
     </row>
     <row r="6" spans="2:16">
       <c r="B6" s="154"/>
-      <c r="C6" s="157" t="s">
-        <v>131</v>
+      <c r="C6" s="199" t="s">
+        <v>113</v>
       </c>
       <c r="D6" s="155"/>
       <c r="E6" s="155"/>
@@ -4929,7 +4934,7 @@
     <row r="7" spans="2:16">
       <c r="B7" s="154"/>
       <c r="C7" s="157" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D7" s="155"/>
       <c r="E7" s="155"/>
@@ -5125,7 +5130,7 @@
       <c r="B18" s="154"/>
       <c r="C18" s="155"/>
       <c r="D18" s="164" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E18" s="155">
         <f>E34</f>
@@ -5149,7 +5154,7 @@
       <c r="B19" s="154"/>
       <c r="C19" s="155"/>
       <c r="D19" s="164" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E19" s="155">
         <f>E35</f>
@@ -5173,13 +5178,13 @@
       <c r="B20" s="154"/>
       <c r="C20" s="155"/>
       <c r="D20" s="164" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E20" s="155">
         <v>6000</v>
       </c>
       <c r="F20" s="169" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G20" s="155"/>
       <c r="H20" s="155"/>
@@ -5306,7 +5311,7 @@
     <row r="28" spans="2:16" s="164" customFormat="1">
       <c r="B28" s="168"/>
       <c r="C28" s="169" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E28" s="169"/>
       <c r="F28" s="169"/>
@@ -5324,12 +5329,12 @@
     <row r="29" spans="2:16" s="164" customFormat="1">
       <c r="B29" s="168"/>
       <c r="C29" s="169" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E29" s="169"/>
       <c r="F29" s="169"/>
       <c r="G29" s="169" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H29" s="169"/>
       <c r="I29" s="169"/>
@@ -5347,7 +5352,7 @@
       <c r="E30" s="169"/>
       <c r="F30" s="169"/>
       <c r="G30" s="169" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H30" s="169"/>
       <c r="I30" s="169"/>
@@ -5365,7 +5370,7 @@
       <c r="E31" s="169"/>
       <c r="F31" s="169"/>
       <c r="G31" s="169" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H31" s="169"/>
       <c r="I31" s="169"/>
@@ -5399,7 +5404,7 @@
       <c r="E33" s="169"/>
       <c r="F33" s="169"/>
       <c r="G33" s="169" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H33" s="169"/>
       <c r="I33" s="169"/>
@@ -5415,7 +5420,7 @@
       <c r="B34" s="168"/>
       <c r="C34" s="169"/>
       <c r="D34" s="169" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E34" s="169">
         <v>42</v>
@@ -5424,7 +5429,7 @@
         <v>3</v>
       </c>
       <c r="G34" s="171" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H34" s="169"/>
       <c r="I34" s="169"/>
@@ -5440,7 +5445,7 @@
       <c r="B35" s="168"/>
       <c r="C35" s="169"/>
       <c r="D35" s="169" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E35" s="169">
         <v>40</v>
@@ -5449,7 +5454,7 @@
         <v>3</v>
       </c>
       <c r="G35" s="171" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H35" s="169"/>
       <c r="I35" s="169"/>
@@ -5466,7 +5471,7 @@
       <c r="C36" s="169"/>
       <c r="E36" s="169"/>
       <c r="G36" s="171" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H36" s="169"/>
       <c r="I36" s="169"/>
@@ -5484,7 +5489,7 @@
       <c r="E37" s="169"/>
       <c r="F37" s="169"/>
       <c r="G37" s="171" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H37" s="169"/>
       <c r="I37" s="169"/>
@@ -5579,7 +5584,7 @@
     <row r="43" spans="2:16">
       <c r="B43" s="154"/>
       <c r="C43" s="157" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E43" s="155"/>
       <c r="F43" s="155"/>
@@ -5733,7 +5738,7 @@
       <c r="B52" s="154"/>
       <c r="C52" s="163"/>
       <c r="D52" s="169" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E52" s="184">
         <f>E51*E66</f>
@@ -5757,7 +5762,7 @@
       <c r="B53" s="154"/>
       <c r="C53" s="155"/>
       <c r="D53" s="164" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E53" s="184">
         <f>E51*E67</f>
@@ -5908,7 +5913,7 @@
     <row r="62" spans="2:17" s="164" customFormat="1">
       <c r="B62" s="168"/>
       <c r="C62" s="169" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E62" s="169"/>
       <c r="F62" s="169"/>
@@ -5927,12 +5932,12 @@
     <row r="63" spans="2:17" s="164" customFormat="1">
       <c r="B63" s="168"/>
       <c r="C63" s="169" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E63" s="169"/>
       <c r="F63" s="169"/>
       <c r="G63" s="169" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H63" s="169"/>
       <c r="I63" s="169"/>
@@ -5985,7 +5990,7 @@
       <c r="B66" s="168"/>
       <c r="C66" s="169"/>
       <c r="D66" s="164" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E66" s="183">
         <f>1/3</f>
@@ -5993,7 +5998,7 @@
       </c>
       <c r="F66" s="169"/>
       <c r="G66" s="164" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H66" s="169"/>
       <c r="I66" s="169"/>
@@ -6010,7 +6015,7 @@
       <c r="B67" s="168"/>
       <c r="C67" s="169"/>
       <c r="D67" s="164" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E67" s="183">
         <f>2/3</f>
@@ -6018,7 +6023,7 @@
       </c>
       <c r="F67" s="169"/>
       <c r="G67" s="164" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H67" s="169"/>
       <c r="I67" s="169"/>
@@ -6037,7 +6042,7 @@
       <c r="E68" s="169"/>
       <c r="F68" s="169"/>
       <c r="G68" s="180" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H68" s="169"/>
       <c r="I68" s="169"/>
@@ -6056,7 +6061,7 @@
       <c r="E69" s="169"/>
       <c r="F69" s="169"/>
       <c r="G69" s="182" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H69" s="169"/>
       <c r="I69" s="169"/>
@@ -6075,7 +6080,7 @@
       <c r="E70" s="169"/>
       <c r="F70" s="169"/>
       <c r="G70" s="181" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H70" s="169"/>
       <c r="I70" s="169"/>
@@ -6094,7 +6099,7 @@
       <c r="E71" s="169"/>
       <c r="F71" s="169"/>
       <c r="G71" s="181" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H71" s="169"/>
       <c r="I71" s="169"/>
@@ -6249,7 +6254,7 @@
         <v>24</v>
       </c>
       <c r="F80" s="157" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G80" s="155"/>
       <c r="H80" s="155"/>
@@ -6365,7 +6370,7 @@
     <row r="87" spans="2:16">
       <c r="B87" s="154"/>
       <c r="C87" s="160" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E87" s="155"/>
       <c r="F87" s="155"/>
@@ -6383,7 +6388,7 @@
     <row r="88" spans="2:16">
       <c r="B88" s="154"/>
       <c r="C88" s="160" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E88" s="155"/>
       <c r="F88" s="155"/>
@@ -6673,7 +6678,7 @@
     <row r="106" spans="2:16">
       <c r="B106" s="154"/>
       <c r="C106" s="160" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E106" s="155">
         <v>1000</v>
@@ -6695,13 +6700,13 @@
     <row r="107" spans="2:16">
       <c r="B107" s="154"/>
       <c r="C107" s="160" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E107" s="155">
         <v>3</v>
       </c>
       <c r="F107" s="160" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G107" s="155"/>
       <c r="H107" s="155"/>

</xml_diff>